<commit_message>
Added KT and ST
</commit_message>
<xml_diff>
--- a/zadaniya.xlsx
+++ b/zadaniya.xlsx
@@ -3070,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3107,56 +3107,56 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>567</v>
+        <v>520</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>501</v>
@@ -3167,36 +3167,36 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>502</v>
@@ -3207,76 +3207,76 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>501</v>
@@ -3287,16 +3287,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>501</v>
@@ -3307,36 +3307,36 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>502</v>
@@ -3347,36 +3347,36 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>367</v>
+        <v>297</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>502</v>
+        <v>482</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>482</v>
@@ -3387,16 +3387,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>482</v>
@@ -3407,96 +3407,96 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>301</v>
+        <v>341</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>481</v>
+        <v>513</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>513</v>
@@ -3507,16 +3507,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>513</v>
@@ -3527,156 +3527,156 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>512</v>
+        <v>485</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>272</v>
+        <v>351</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>351</v>
+        <v>277</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>501</v>
+        <v>470</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>470</v>
+        <v>485</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>485</v>
@@ -3687,136 +3687,136 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>470</v>
+        <v>494</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>494</v>
+        <v>470</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>470</v>
+        <v>512</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>512</v>
+        <v>467</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>260</v>
+        <v>376</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>55</v>
+        <v>171</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>467</v>
+        <v>485</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>485</v>
@@ -3827,56 +3827,56 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>377</v>
+        <v>302</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>302</v>
+        <v>262</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>483</v>
@@ -3887,16 +3887,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>483</v>
@@ -3907,36 +3907,36 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>264</v>
+        <v>310</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>481</v>
@@ -3947,122 +3947,122 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>481</v>
+        <v>512</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>512</v>
+        <v>492</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>492</v>
+        <v>515</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>513</v>
+        <v>485</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>485</v>
+        <v>503</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>